<commit_message>
add feature and refactoring
</commit_message>
<xml_diff>
--- a/xls/demo.xlsx
+++ b/xls/demo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>S1</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -85,6 +85,14 @@
   </si>
   <si>
     <t>怪物名字</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>特点1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>特点2</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1013,10 +1021,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1032,7 +1040,7 @@
     <col min="10" max="10" width="31.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:12">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -1063,8 +1071,14 @@
       <c r="J1" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:12">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1095,8 +1109,14 @@
       <c r="J2">
         <v>1</v>
       </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>2</v>
+      </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:12">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1127,8 +1147,14 @@
       <c r="J3">
         <v>2</v>
       </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>2</v>
+      </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:12">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1159,8 +1185,14 @@
       <c r="J4">
         <v>3</v>
       </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>2</v>
+      </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:12">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1191,8 +1223,14 @@
       <c r="J5">
         <v>4</v>
       </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>2</v>
+      </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:12">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1222,6 +1260,12 @@
       </c>
       <c r="J6">
         <v>5</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>